<commit_message>
chat bot 연동 test 1
</commit_message>
<xml_diff>
--- a/Develop/juwhan/서버/ChatBot/chatbot_data_find.xlsx
+++ b/Develop/juwhan/서버/ChatBot/chatbot_data_find.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTL\Desktop\GitHub\Dokkaebi_Box\Develop\jaehyun\test\chatbotTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTL\Desktop\GitHub\Dokkaebi_Box\Develop\jaehyun\test\ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5812BCC-A591-4368-AFFE-2AD989965211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCC4FE3-9932-4BC6-92E1-D1B92FD645C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52476728-7820-42B9-9744-745D88BAFB62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52476728-7820-42B9-9744-745D88BAFB62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>request</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,58 +44,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>분실물 맡기러 왔어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물건 맡기러 왔어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분실물 찾으러 왔어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분실물|찾으러</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물건 찾으러 왔어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물건|찾으러</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>response</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물건 맡기고 싶어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물건|맡기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분실물|맡기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>맡기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어떤 종류의 물건인가요? (휴대폰/지갑/기타)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>맡기러왔어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>휴대폰이야</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>휴대폰을 맡기러 오셨군요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>폰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,15 +96,122 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물건</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분실물을 맡기러 오셨나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분실물</t>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cellphone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>wallet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전화기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드지갑이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드지갑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반지갑이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반지갑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>명함지갑이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>명함지갑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에어팟이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에어팟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버즈야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이어폰이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이어폰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화장품이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화장품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11월 3일 10시 47분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월|일|시|분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>휴대폰을 찾으러 오셨군요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑을 찾으러 오셨군요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(기타)을(를) 찾으러 오셨군요?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1373A46-C6FB-4AE1-AE85-9F8568CCDA82}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -534,7 +589,7 @@
     <col min="3" max="3" width="40.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,161 +597,279 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>